<commit_message>
Add more dashboard panels
</commit_message>
<xml_diff>
--- a/monitoring-stack/docs/metric_mapping.xlsx
+++ b/monitoring-stack/docs/metric_mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t xml:space="preserve">Physical Host</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">CPU</t>
   </si>
   <si>
-    <t xml:space="preserve">usage_idle*</t>
+    <t xml:space="preserve">usage_idle</t>
   </si>
   <si>
     <t xml:space="preserve">Valor zero em todos os containers</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">io.stat→wbytes</t>
   </si>
   <si>
-    <t xml:space="preserve">io_time</t>
+    <t xml:space="preserve">io_time – não preciso usar, pois já tenho o io_util</t>
   </si>
   <si>
     <t xml:space="preserve">io.stat→time</t>
@@ -169,7 +169,10 @@
     <t xml:space="preserve">faltam</t>
   </si>
   <si>
-    <t xml:space="preserve">inputs.net</t>
+    <t xml:space="preserve">cpu.pressure ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">io.pressure ?</t>
   </si>
 </sst>
 </file>
@@ -217,14 +220,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00A933"/>
-        <bgColor rgb="FF008000"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -356,10 +359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,10 +399,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -407,10 +410,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -418,10 +421,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -434,18 +437,18 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -453,10 +456,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -464,10 +467,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -477,10 +480,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -488,10 +491,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
@@ -499,10 +502,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="0" t="s">
@@ -515,10 +518,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="0" t="s">
@@ -526,10 +529,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="0" t="s">
@@ -537,10 +540,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="0" t="s">
@@ -548,10 +551,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -564,7 +567,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="0" t="s">
@@ -575,7 +578,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="0" t="s">
@@ -586,7 +589,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="0" t="s">
@@ -597,7 +600,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="0" t="s">
@@ -611,43 +614,15 @@
       <c r="A31" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="0" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
-        <v>47</v>
+      <c r="C34" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add network+processes metrics to virtual devices
</commit_message>
<xml_diff>
--- a/monitoring-stack/docs/metric_mapping.xlsx
+++ b/monitoring-stack/docs/metric_mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t xml:space="preserve">Physical Host</t>
   </si>
@@ -154,9 +154,6 @@
     <t xml:space="preserve">running</t>
   </si>
   <si>
-    <t xml:space="preserve">Requiresprocstat+ PID namespace</t>
-  </si>
-  <si>
     <t xml:space="preserve">Not cgroup-native</t>
   </si>
   <si>
@@ -166,13 +163,37 @@
     <t xml:space="preserve">zombies</t>
   </si>
   <si>
-    <t xml:space="preserve">faltam</t>
+    <t xml:space="preserve">Net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bytes Received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bytes Sent</t>
   </si>
   <si>
     <t xml:space="preserve">cpu.pressure ? </t>
   </si>
   <si>
+    <t xml:space="preserve">Packets Received</t>
+  </si>
+  <si>
     <t xml:space="preserve">io.pressure ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packets Sent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error Out</t>
   </si>
 </sst>
 </file>
@@ -359,13 +380,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="46.71"/>
@@ -570,59 +591,119 @@
       <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B32" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C33" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="C34" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add questions + update diskio metrics & dashboard
</commit_message>
<xml_diff>
--- a/monitoring-stack/docs/metric_mapping.xlsx
+++ b/monitoring-stack/docs/metric_mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t xml:space="preserve">Physical Host</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requires host-level monitoring</t>
   </si>
   <si>
     <t xml:space="preserve">inodes_free</t>
@@ -383,10 +380,10 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="46.71"/>
@@ -508,7 +505,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,53 +516,53 @@
         <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C21" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>9</v>
@@ -573,10 +570,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>9</v>
@@ -584,29 +581,29 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,93 +614,93 @@
         <v>19</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>